<commit_message>
Erstellung der algorithmen zum befüllen der Sheets Anpassung
</commit_message>
<xml_diff>
--- a/Evaluation/FLStandard/Version3.xlsx
+++ b/Evaluation/FLStandard/Version3.xlsx
@@ -680,6 +680,9 @@
       <c r="C5" t="n">
         <v>92.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -691,6 +694,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -1036,6 +1042,9 @@
       <c r="C5" t="n">
         <v>93.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -1047,6 +1056,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -1392,6 +1404,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.91666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -1403,6 +1418,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -1748,6 +1766,9 @@
       <c r="C5" t="n">
         <v>94.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -1759,6 +1780,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.66666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -2104,6 +2128,9 @@
       <c r="C5" t="n">
         <v>94</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -2115,6 +2142,9 @@
       </c>
       <c r="C6" t="n">
         <v>95</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.58333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -2460,6 +2490,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -2471,6 +2504,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.25</v>
       </c>
     </row>
     <row r="7">
@@ -2816,6 +2852,9 @@
       <c r="C5" t="n">
         <v>94.08333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -2827,6 +2866,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -3172,6 +3214,9 @@
       <c r="C5" t="n">
         <v>93.08333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>96.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -3183,6 +3228,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.58333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -3528,6 +3576,9 @@
       <c r="C5" t="n">
         <v>93.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -3539,6 +3590,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94</v>
       </c>
     </row>
     <row r="7">
@@ -3884,6 +3938,9 @@
       <c r="C5" t="n">
         <v>93.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -3895,6 +3952,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.91666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -4240,6 +4300,9 @@
       <c r="C5" t="n">
         <v>94.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -4251,6 +4314,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -4596,6 +4662,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -4607,6 +4676,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -4952,6 +5024,9 @@
       <c r="C5" t="n">
         <v>94.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -4963,6 +5038,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -5308,6 +5386,9 @@
       <c r="C5" t="n">
         <v>93.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -5319,6 +5400,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>93.83333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -5664,6 +5748,9 @@
       <c r="C5" t="n">
         <v>94.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -5675,6 +5762,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.83333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.75</v>
       </c>
     </row>
     <row r="7">
@@ -6020,6 +6110,9 @@
       <c r="C5" t="n">
         <v>0.1878712517209351</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.08478690500487573</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -6031,6 +6124,9 @@
       </c>
       <c r="C6" t="n">
         <v>0.1604767544195056</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1982489372603595</v>
       </c>
     </row>
     <row r="7">
@@ -6376,6 +6472,9 @@
       <c r="C5" t="n">
         <v>94.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.66666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -6387,6 +6486,9 @@
       </c>
       <c r="C6" t="n">
         <v>95</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.25</v>
       </c>
     </row>
     <row r="7">
@@ -6732,6 +6834,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.25</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -6743,6 +6848,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>96.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -7088,6 +7196,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.66666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -7099,6 +7210,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="7">
@@ -7444,6 +7558,9 @@
       <c r="C5" t="n">
         <v>92.75</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -7455,6 +7572,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -7800,6 +7920,9 @@
       <c r="C5" t="n">
         <v>94.08333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.25</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -7810,6 +7933,9 @@
         <v>93.66666666666667</v>
       </c>
       <c r="C6" t="n">
+        <v>95.25</v>
+      </c>
+      <c r="D6" t="n">
         <v>95.25</v>
       </c>
     </row>
@@ -8156,6 +8282,9 @@
       <c r="C5" t="n">
         <v>94.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -8167,6 +8296,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.91666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -8512,6 +8644,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -8523,6 +8658,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -8868,6 +9006,9 @@
       <c r="C5" t="n">
         <v>94.83333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.91666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -8879,6 +9020,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.66666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -9224,6 +9368,9 @@
       <c r="C5" t="n">
         <v>93.75</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -9235,6 +9382,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -9580,6 +9730,9 @@
       <c r="C5" t="n">
         <v>95</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -9591,6 +9744,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.91666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -9936,6 +10092,9 @@
       <c r="C5" t="n">
         <v>0.005948876455081336</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.006340112332996796</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -9947,6 +10106,9 @@
       </c>
       <c r="C6" t="n">
         <v>0.005125088675196457</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.005786698634765343</v>
       </c>
     </row>
     <row r="7">
@@ -10292,6 +10454,9 @@
       <c r="C5" t="n">
         <v>94.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -10303,6 +10468,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>96.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -10648,6 +10816,9 @@
       <c r="C5" t="n">
         <v>95.16666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.66666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -10659,6 +10830,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -11004,6 +11178,9 @@
       <c r="C5" t="n">
         <v>94</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -11015,6 +11192,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -11360,6 +11540,9 @@
       <c r="C5" t="n">
         <v>94.16666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -11371,6 +11554,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.5</v>
       </c>
     </row>
     <row r="7">
@@ -11716,6 +11902,9 @@
       <c r="C5" t="n">
         <v>93.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -11727,6 +11916,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.58333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -12072,6 +12264,9 @@
       <c r="C5" t="n">
         <v>94.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -12083,6 +12278,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>93.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -12428,6 +12626,9 @@
       <c r="C5" t="n">
         <v>95.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -12439,6 +12640,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -12784,6 +12988,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -12795,6 +13002,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.58333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -13140,6 +13350,9 @@
       <c r="C5" t="n">
         <v>94.75</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -13151,6 +13364,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>93.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -13496,6 +13712,9 @@
       <c r="C5" t="n">
         <v>94.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.66666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -13507,6 +13726,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.25</v>
       </c>
     </row>
     <row r="7">
@@ -13852,6 +14074,9 @@
       <c r="C5" t="n">
         <v>95.23999999999999</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.52</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -13863,6 +14088,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.81999999999999</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.79000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -14208,6 +14436,9 @@
       <c r="C5" t="n">
         <v>94.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -14219,6 +14450,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>93.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -14564,6 +14798,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -14575,6 +14812,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>93.83333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -14920,6 +15160,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.25</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -14931,6 +15174,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.83333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -15276,6 +15522,9 @@
       <c r="C5" t="n">
         <v>94.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -15287,6 +15536,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>92.66666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -15632,6 +15884,9 @@
       <c r="C5" t="n">
         <v>94.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.25</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -15643,6 +15898,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -15988,6 +16246,9 @@
       <c r="C5" t="n">
         <v>94.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -15999,6 +16260,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -16344,6 +16608,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -16355,6 +16622,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -16700,6 +16970,9 @@
       <c r="C5" t="n">
         <v>94.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -16711,6 +16984,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -17056,6 +17332,9 @@
       <c r="C5" t="n">
         <v>94.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -17067,6 +17346,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -17412,6 +17694,9 @@
       <c r="C5" t="n">
         <v>94.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -17423,6 +17708,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -17768,6 +18056,9 @@
       <c r="C5" t="n">
         <v>93.16666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -17779,6 +18070,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.75</v>
       </c>
     </row>
     <row r="7">
@@ -18124,6 +18418,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -18135,6 +18432,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.5</v>
       </c>
     </row>
     <row r="7">
@@ -18480,6 +18780,9 @@
       <c r="C5" t="n">
         <v>95.16666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>96.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -18491,6 +18794,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.75</v>
       </c>
     </row>
     <row r="7">
@@ -18836,6 +19142,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -18847,6 +19156,9 @@
       </c>
       <c r="C6" t="n">
         <v>96</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -19192,6 +19504,9 @@
       <c r="C5" t="n">
         <v>93.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.33333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -19203,6 +19518,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.25</v>
       </c>
     </row>
     <row r="7">
@@ -19548,6 +19866,9 @@
       <c r="C5" t="n">
         <v>93.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -19559,6 +19880,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.25</v>
       </c>
     </row>
     <row r="7">
@@ -19904,6 +20228,9 @@
       <c r="C5" t="n">
         <v>94.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -19915,6 +20242,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.25</v>
       </c>
     </row>
     <row r="7">
@@ -20260,6 +20590,9 @@
       <c r="C5" t="n">
         <v>93.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.91666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -20271,6 +20604,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -20616,6 +20952,9 @@
       <c r="C5" t="n">
         <v>95.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.91666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -20627,6 +20966,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.75</v>
       </c>
     </row>
     <row r="7">
@@ -20972,6 +21314,9 @@
       <c r="C5" t="n">
         <v>93.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -20983,6 +21328,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.83333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.75</v>
       </c>
     </row>
     <row r="7">
@@ -21328,6 +21676,9 @@
       <c r="C5" t="n">
         <v>94.75</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.66666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -21339,6 +21690,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -21684,6 +22038,9 @@
       <c r="C5" t="n">
         <v>94</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.91666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -21694,6 +22051,9 @@
         <v>95</v>
       </c>
       <c r="C6" t="n">
+        <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
         <v>95.41666666666667</v>
       </c>
     </row>
@@ -22040,6 +22400,9 @@
       <c r="C5" t="n">
         <v>94.08333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -22051,6 +22414,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -22396,6 +22762,9 @@
       <c r="C5" t="n">
         <v>94.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.33333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -22407,6 +22776,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.5</v>
       </c>
     </row>
     <row r="7">
@@ -22752,6 +23124,9 @@
       <c r="C5" t="n">
         <v>94.83333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>96.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -22763,6 +23138,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.83333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -23108,6 +23486,9 @@
       <c r="C5" t="n">
         <v>93.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.25</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -23119,6 +23500,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.25</v>
       </c>
     </row>
     <row r="7">
@@ -23464,6 +23848,9 @@
       <c r="C5" t="n">
         <v>93.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.33333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -23475,6 +23862,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -23820,6 +24210,9 @@
       <c r="C5" t="n">
         <v>93</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -23831,6 +24224,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.75</v>
       </c>
     </row>
     <row r="7">
@@ -24176,6 +24572,9 @@
       <c r="C5" t="n">
         <v>92.16666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -24187,6 +24586,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="7">
@@ -24532,6 +24934,9 @@
       <c r="C5" t="n">
         <v>93.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.25</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -24543,6 +24948,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.75</v>
       </c>
     </row>
     <row r="7">
@@ -24888,6 +25296,9 @@
       <c r="C5" t="n">
         <v>92.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -24899,6 +25310,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -25244,6 +25658,9 @@
       <c r="C5" t="n">
         <v>93.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -25255,6 +25672,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -25600,6 +26020,9 @@
       <c r="C5" t="n">
         <v>93.75</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -25611,6 +26034,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.5</v>
       </c>
     </row>
     <row r="7">
@@ -25956,6 +26382,9 @@
       <c r="C5" t="n">
         <v>92.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -25967,6 +26396,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.83333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -26312,6 +26744,9 @@
       <c r="C5" t="n">
         <v>92.83333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -26323,6 +26758,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.25</v>
       </c>
     </row>
     <row r="7">
@@ -26668,6 +27106,9 @@
       <c r="C5" t="n">
         <v>94.33333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.66666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -26679,6 +27120,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.5</v>
       </c>
     </row>
     <row r="7">
@@ -27024,6 +27468,9 @@
       <c r="C5" t="n">
         <v>91.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -27035,6 +27482,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -27380,6 +27830,9 @@
       <c r="C5" t="n">
         <v>92.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -27391,6 +27844,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -27736,6 +28192,9 @@
       <c r="C5" t="n">
         <v>94.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -27747,6 +28206,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.91666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.5</v>
       </c>
     </row>
     <row r="7">
@@ -28092,6 +28554,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -28103,6 +28568,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.66666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -28448,6 +28916,9 @@
       <c r="C5" t="n">
         <v>95.16666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -28459,6 +28930,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -28804,6 +29278,9 @@
       <c r="C5" t="n">
         <v>93.08333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -28815,6 +29292,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.41666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -29160,6 +29640,9 @@
       <c r="C5" t="n">
         <v>93.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -29171,6 +29654,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.83333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -29516,6 +30002,9 @@
       <c r="C5" t="n">
         <v>93.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -29527,6 +30016,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -29872,6 +30364,9 @@
       <c r="C5" t="n">
         <v>94.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -29883,6 +30378,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.25</v>
       </c>
     </row>
     <row r="7">
@@ -30228,6 +30726,9 @@
       <c r="C5" t="n">
         <v>94.66666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -30239,6 +30740,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -30584,6 +31088,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.33333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -30595,6 +31102,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="7">
@@ -30940,6 +31450,9 @@
       <c r="C5" t="n">
         <v>94.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.91666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -30951,6 +31464,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.25</v>
       </c>
     </row>
     <row r="7">
@@ -31296,6 +31812,9 @@
       <c r="C5" t="n">
         <v>93.08333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -31307,6 +31826,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="7">
@@ -31652,6 +32174,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -31663,6 +32188,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.66666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.83333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -32008,6 +32536,9 @@
       <c r="C5" t="n">
         <v>94.16666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -32019,6 +32550,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -32364,6 +32898,9 @@
       <c r="C5" t="n">
         <v>95.25</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -32375,6 +32912,9 @@
       </c>
       <c r="C6" t="n">
         <v>96</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.58333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -32720,6 +33260,9 @@
       <c r="C5" t="n">
         <v>93.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -32731,6 +33274,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -33076,6 +33622,9 @@
       <c r="C5" t="n">
         <v>93.83333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -33087,6 +33636,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -33432,6 +33984,9 @@
       <c r="C5" t="n">
         <v>93.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -33443,6 +33998,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.41666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -33788,6 +34346,9 @@
       <c r="C5" t="n">
         <v>94.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -33799,6 +34360,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.91666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -34144,6 +34708,9 @@
       <c r="C5" t="n">
         <v>94.75</v>
       </c>
+      <c r="D5" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -34155,6 +34722,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -34500,6 +35070,9 @@
       <c r="C5" t="n">
         <v>94.41666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.83333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -34511,6 +35084,9 @@
       </c>
       <c r="C6" t="n">
         <v>96</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.58333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -34856,6 +35432,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.08333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -34867,6 +35446,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -35212,6 +35794,9 @@
       <c r="C5" t="n">
         <v>93.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>93.91666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -35223,6 +35808,9 @@
       </c>
       <c r="C6" t="n">
         <v>94.58333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -35568,6 +36156,9 @@
       <c r="C5" t="n">
         <v>94.83333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -35579,6 +36170,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.25</v>
       </c>
     </row>
     <row r="7">
@@ -35924,6 +36518,9 @@
       <c r="C5" t="n">
         <v>94.91666666666667</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -35935,6 +36532,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.08333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -36280,6 +36880,9 @@
       <c r="C5" t="n">
         <v>95.58333333333333</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.41666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -36291,6 +36894,9 @@
       </c>
       <c r="C6" t="n">
         <v>96.16666666666667</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.16666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -36636,6 +37242,9 @@
       <c r="C5" t="n">
         <v>93.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>94.16666666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -36647,6 +37256,9 @@
       </c>
       <c r="C6" t="n">
         <v>95.33333333333333</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94.33333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -36992,6 +37604,9 @@
       <c r="C5" t="n">
         <v>94.5</v>
       </c>
+      <c r="D5" t="n">
+        <v>95.58333333333333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -37003,6 +37618,9 @@
       </c>
       <c r="C6" t="n">
         <v>95</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95.66666666666667</v>
       </c>
     </row>
     <row r="7">

</xml_diff>